<commit_message>
feat: registro de data do relatorio
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/model.xlsx
+++ b/src/main/resources/excel/model.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28803"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A484066D-9595-488C-B544-801C1EBF0EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{077587FB-FAA1-425F-9466-BCB391D39D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+  <si>
+    <t>Faturamento Mensal (estimado)</t>
+  </si>
+  <si>
+    <t>Quantidade gasta em Lotes</t>
+  </si>
+  <si>
+    <t>Quantidade de produtos sem saida registrada</t>
+  </si>
   <si>
     <t>Produtos</t>
   </si>
@@ -125,8 +134,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -259,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -267,6 +277,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -285,16 +312,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -304,9 +321,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -316,10 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,6 +346,872 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Baixas de Estoque'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Baixas de Estoque'!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-BB36-48CF-A0B5-7A6E6357B776}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="565783560"/>
+        <c:axId val="856331272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="565783560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="856331272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="856331272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="565783560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75FF1CB3-50FA-D0C9-E24A-245303CC261C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -654,13 +1531,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="32"/>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -680,60 +1580,60 @@
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="9"/>
+      <c r="A1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -755,61 +1655,61 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="15" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="9" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.5703125" customWidth="1"/>
     <col min="10" max="10" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12"/>
+      <c r="A1" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="14" t="s">
         <v>16</v>
       </c>
+      <c r="B2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="E2" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -840,37 +1740,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="A1" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="23" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>19</v>
+      <c r="B2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -885,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92F93FC-EE62-4839-9E37-E57063B6AD63}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -896,42 +1796,42 @@
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27"/>
+      <c r="A1" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="29" t="s">
+      <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>19</v>
+      <c r="B2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: excel model, gráfico de produtos de saida
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/model.xlsx
+++ b/src/main/resources/excel/model.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28803"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{077587FB-FAA1-425F-9466-BCB391D39D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17C10FF7-FD92-493F-9D42-ED278031300E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,7 +136,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -294,6 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -330,7 +331,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,6 +363,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Saida por Produtos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -400,19 +425,14 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="5"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Baixas de Estoque'!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Produtos</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -420,18 +440,41 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Baixas de Estoque'!$C$3:$C$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="98"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Baixas de Estoque'!$B$3:$G$3</c:f>
+              <c:f>'Baixas de Estoque'!$G$3:$G$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="98"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-BB36-48CF-A0B5-7A6E6357B776}"/>
+              <c16:uniqueId val="{0000000C-16B4-4441-B0C2-8CB7CAAF2477}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -443,18 +486,19 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
+        <c:gapWidth val="104"/>
         <c:overlap val="-27"/>
-        <c:axId val="565783560"/>
-        <c:axId val="856331272"/>
+        <c:axId val="9788423"/>
+        <c:axId val="9790471"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565783560"/>
+        <c:axId val="9788423"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -491,7 +535,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="856331272"/>
+        <c:crossAx val="9790471"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -499,7 +543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="856331272"/>
+        <c:axId val="9790471"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -535,7 +579,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -550,9 +594,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565783560"/>
+        <c:crossAx val="9788423"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -562,37 +607,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1177,23 +1191,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75FF1CB3-50FA-D0C9-E24A-245303CC261C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0387A4F7-2F9C-D57C-B72F-2CB28B60AD3E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1531,29 +1545,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="32"/>
+    <row r="1" spans="1:2">
+      <c r="A1" s="20"/>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <f>SUM(Lotes!H3,Lotes!H100)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1587,19 +1607,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
@@ -1667,18 +1687,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
@@ -1740,15 +1760,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="13" t="s">
@@ -1785,8 +1805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92F93FC-EE62-4839-9E37-E57063B6AD63}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1801,15 +1821,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="16" t="s">

</xml_diff>

<commit_message>
fix: relatorio dash kpi
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/model.xlsx
+++ b/src/main/resources/excel/model.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28803"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17C10FF7-FD92-493F-9D42-ED278031300E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E015E53-19BE-48EB-8B3E-271D1B2FF1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+  <si>
+    <t>Relatório gerado em:</t>
+  </si>
   <si>
     <t>Faturamento Mensal (estimado)</t>
   </si>
@@ -134,9 +137,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -294,7 +296,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -331,6 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1548,7 +1550,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1557,16 +1559,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="20"/>
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <f>SUM(Lotes!H3,Lotes!H100)</f>
@@ -1575,7 +1580,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1607,53 +1612,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75">
-      <c r="A1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="23"/>
+      <c r="A1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1687,49 +1692,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26"/>
+      <c r="A1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1760,37 +1765,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
+      <c r="A1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1821,37 +1826,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
+      <c r="A1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge main into aws (#4)
* feat: registro de data do relatorio

* feat: excel model, gráfico de produtos de saida

* fix: Atualizando produto para usar no método de deletar

* feat: delete marca

* feat: delete subtipo

* feat: delete tipo

* feat: retornando id de saidaEstoque

* fix: relatorio dash kpi

* feat: endpoint de buscar lotes por produto

* feat: atualizando estoque de produtos com lote status entregue

* feat: deletando loteprodutos existentes ao atualizar

* refactor: Passando nova lista de produtos, marca e tipos

---------

Co-authored-by: Kauan-deAlmeida <kauan.almeida@sptech.school>
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/model.xlsx
+++ b/src/main/resources/excel/model.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28803"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A484066D-9595-488C-B544-801C1EBF0EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E015E53-19BE-48EB-8B3E-271D1B2FF1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+  <si>
+    <t>Relatório gerado em:</t>
+  </si>
+  <si>
+    <t>Faturamento Mensal (estimado)</t>
+  </si>
+  <si>
+    <t>Quantidade gasta em Lotes</t>
+  </si>
+  <si>
+    <t>Quantidade de produtos sem saida registrada</t>
+  </si>
   <si>
     <t>Produtos</t>
   </si>
@@ -126,7 +138,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -259,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -267,6 +279,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -285,16 +314,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -304,9 +323,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -316,10 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,6 +348,886 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Saida por Produtos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Produtos</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Baixas de Estoque'!$C$3:$C$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="98"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Baixas de Estoque'!$G$3:$G$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="98"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-16B4-4441-B0C2-8CB7CAAF2477}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="104"/>
+        <c:overlap val="-27"/>
+        <c:axId val="9788423"/>
+        <c:axId val="9790471"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="9788423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="9790471"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="9790471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="9788423"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0387A4F7-2F9C-D57C-B72F-2CB28B60AD3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -654,13 +1547,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>SUM(Lotes!H3,Lotes!H100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -680,60 +1605,60 @@
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="9"/>
+      <c r="A1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -755,61 +1680,61 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="15" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="9" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.5703125" customWidth="1"/>
     <col min="10" max="10" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="12"/>
+      <c r="A1" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -840,37 +1765,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="A1" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="23" t="s">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>19</v>
+      <c r="B2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -885,8 +1810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92F93FC-EE62-4839-9E37-E57063B6AD63}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -896,42 +1821,42 @@
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27"/>
+      <c r="A1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="29" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>19</v>
+      <c r="B2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add excel dash kpis
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/model.xlsx
+++ b/src/main/resources/excel/model.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28908"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E015E53-19BE-48EB-8B3E-271D1B2FF1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B91E868-CA9D-45FE-BC6A-D9EB6A711CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1193,16 +1193,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1550,7 +1550,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1559,7 +1559,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7"/>
@@ -1568,20 +1568,19 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="11"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <f>SUM(Lotes!H3,Lotes!H100)</f>
-        <v>0</v>
-      </c>
+      <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>